<commit_message>
update climate categories by number
</commit_message>
<xml_diff>
--- a/ChilwaBasin_DataAnalysis_032024/Dataset/ChilwaBasin_AgricultureClimateDataset_04052024.xlsx
+++ b/ChilwaBasin_DataAnalysis_032024/Dataset/ChilwaBasin_AgricultureClimateDataset_04052024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali\Documents\GitHub\ChilwaBasin\ChilwaBasin_DataAnalysis_032024\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0006FC1C-FF06-41C8-8C43-41311D1F728E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34106FDA-4B1E-47F3-BEE5-D3B276688C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{C89A1868-8892-4AF7-9BC8-1A55A47CDD85}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Year</t>
   </si>
@@ -156,21 +156,6 @@
   </si>
   <si>
     <t>UREATotal_T</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Dry</t>
-  </si>
-  <si>
-    <t>Wet</t>
-  </si>
-  <si>
-    <t>Extreme Dry</t>
-  </si>
-  <si>
-    <t>Extreme Wet</t>
   </si>
   <si>
     <t>ClimateSatellite</t>
@@ -635,7 +620,7 @@
   <dimension ref="A1:AP64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -688,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -815,11 +800,11 @@
       <c r="A2">
         <v>2010</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
       </c>
       <c r="D2">
         <v>244.3</v>
@@ -931,11 +916,11 @@
       <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
       </c>
       <c r="D3">
         <v>251.8</v>
@@ -1047,11 +1032,11 @@
       <c r="A4">
         <v>2012</v>
       </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
       <c r="D4">
         <v>149.5</v>
@@ -1163,11 +1148,11 @@
       <c r="A5">
         <v>2013</v>
       </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
       </c>
       <c r="D5">
         <v>331</v>
@@ -1291,11 +1276,11 @@
       <c r="A6">
         <v>2014</v>
       </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
       </c>
       <c r="D6">
         <v>79.5</v>
@@ -1419,11 +1404,11 @@
       <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
       </c>
       <c r="D7">
         <v>140</v>
@@ -1547,11 +1532,11 @@
       <c r="A8">
         <v>2016</v>
       </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
       </c>
       <c r="D8">
         <v>187.5</v>
@@ -1675,11 +1660,11 @@
       <c r="A9">
         <v>2017</v>
       </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
       </c>
       <c r="D9">
         <v>190</v>
@@ -1803,11 +1788,11 @@
       <c r="A10">
         <v>2018</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="D10">
         <v>271.5</v>
@@ -1931,8 +1916,8 @@
       <c r="A11">
         <v>2019</v>
       </c>
-      <c r="B11" t="s">
-        <v>44</v>
+      <c r="B11">
+        <v>5</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2056,8 +2041,8 @@
       <c r="A12">
         <v>2020</v>
       </c>
-      <c r="B12" t="s">
-        <v>43</v>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="D12">
         <v>238</v>
@@ -2181,8 +2166,8 @@
       <c r="A13">
         <v>2021</v>
       </c>
-      <c r="B13" t="s">
-        <v>42</v>
+      <c r="B13">
+        <v>4</v>
       </c>
       <c r="D13">
         <v>260.5</v>
@@ -2306,8 +2291,8 @@
       <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
+      <c r="B14">
+        <v>5</v>
       </c>
       <c r="D14">
         <v>186</v>

</xml_diff>